<commit_message>
Updated GOMS operational sequence
</commit_message>
<xml_diff>
--- a/GOMS.xlsx
+++ b/GOMS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="440" windowWidth="19200" windowHeight="23560" tabRatio="500"/>
+    <workbookView xWindow="19200" yWindow="440" windowWidth="19200" windowHeight="23560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Comp Performer" sheetId="1" r:id="rId1"/>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1128,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G1:H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1200,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E26" si="0">IF(ISNUMBER(VLOOKUP(C3,$G$2:$H$6,2,FALSE)), VLOOKUP(C3,$G$2:$H$6,2,FALSE) * D3, "t")</f>
+        <f t="shared" ref="E3:E19" si="0">IF(ISNUMBER(VLOOKUP(C3,$G$2:$H$6,2,FALSE)), VLOOKUP(C3,$G$2:$H$6,2,FALSE) * D3, "t")</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1212,7 +1212,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f t="shared" ref="A4:A26" si="1">A3+1</f>
+        <f t="shared" ref="A4:A19" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1297,11 +1297,11 @@
         <v>21</v>
       </c>
       <c r="D7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1449,11 +1449,11 @@
         <v>21</v>
       </c>
       <c r="D15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>